<commit_message>
removed ones from correlation map in MLR
</commit_message>
<xml_diff>
--- a/results/ML/MLR_cat_enroll_vs_Desertor/backwardElimination.xlsx
+++ b/results/ML/MLR_cat_enroll_vs_Desertor/backwardElimination.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\MLR_cat_enroll_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CDC04E-6102-49A9-9873-B1234F5BA2DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A120CB7E-57F8-470A-AC60-1D5C9DCF85A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,13 +28,14 @@
     <sheet name="6" sheetId="13" r:id="rId13"/>
     <sheet name="5" sheetId="14" r:id="rId14"/>
     <sheet name="4" sheetId="15" r:id="rId15"/>
+    <sheet name="3" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="36">
   <si>
     <t>Columns on Logic</t>
   </si>
@@ -102,7 +103,7 @@
 Model:                            OLS   Adj. R-squared:                  0.033
 Method:                 Least Squares   F-statistic:                     2.019
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00780
-Time:                        22:58:29   Log-Likelihood:                -322.70
+Time:                        23:07:16   Log-Likelihood:                -322.70
 No. Observations:                 537   AIC:                             683.4
 Df Residuals:                     518   BIC:                             764.8
 Df Model:                          18                                         
@@ -145,7 +146,7 @@
 Model:                            OLS   Adj. R-squared:                  0.035
 Method:                 Least Squares   F-statistic:                     2.142
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00504
-Time:                        22:58:29   Log-Likelihood:                -322.71
+Time:                        23:07:16   Log-Likelihood:                -322.71
 No. Observations:                 537   AIC:                             681.4
 Df Residuals:                     519   BIC:                             758.6
 Df Model:                          17                                         
@@ -187,7 +188,7 @@
 Model:                            OLS   Adj. R-squared:                  0.037
 Method:                 Least Squares   F-statistic:                     2.280
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00316
-Time:                        22:58:29   Log-Likelihood:                -322.71
+Time:                        23:07:16   Log-Likelihood:                -322.71
 No. Observations:                 537   AIC:                             679.4
 Df Residuals:                     520   BIC:                             752.3
 Df Model:                          16                                         
@@ -228,7 +229,7 @@
 Model:                            OLS   Adj. R-squared:                  0.039
 Method:                 Least Squares   F-statistic:                     2.434
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00194
-Time:                        22:58:29   Log-Likelihood:                -322.73
+Time:                        23:07:16   Log-Likelihood:                -322.73
 No. Observations:                 537   AIC:                             677.5
 Df Residuals:                     521   BIC:                             746.0
 Df Model:                          15                                         
@@ -268,7 +269,7 @@
 Model:                            OLS   Adj. R-squared:                  0.040
 Method:                 Least Squares   F-statistic:                     2.581
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00131
-Time:                        22:58:29   Log-Likelihood:                -322.94
+Time:                        23:07:16   Log-Likelihood:                -322.94
 No. Observations:                 537   AIC:                             675.9
 Df Residuals:                     522   BIC:                             740.2
 Df Model:                          14                                         
@@ -307,7 +308,7 @@
 Model:                            OLS   Adj. R-squared:                  0.040
 Method:                 Least Squares   F-statistic:                     2.718
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):           0.000992
-Time:                        22:58:29   Log-Likelihood:                -323.35
+Time:                        23:07:16   Log-Likelihood:                -323.35
 No. Observations:                 537   AIC:                             674.7
 Df Residuals:                     523   BIC:                             734.7
 Df Model:                          13                                         
@@ -345,7 +346,7 @@
 Model:                            OLS   Adj. R-squared:                  0.041
 Method:                 Least Squares   F-statistic:                     2.925
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):           0.000605
-Time:                        22:58:29   Log-Likelihood:                -323.50
+Time:                        23:07:16   Log-Likelihood:                -323.50
 No. Observations:                 537   AIC:                             673.0
 Df Residuals:                     524   BIC:                             728.7
 Df Model:                          12                                         
@@ -382,7 +383,7 @@
 Model:                            OLS   Adj. R-squared:                  0.040
 Method:                 Least Squares   F-statistic:                     3.052
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):           0.000562
-Time:                        22:58:29   Log-Likelihood:                -324.26
+Time:                        23:07:16   Log-Likelihood:                -324.26
 No. Observations:                 537   AIC:                             672.5
 Df Residuals:                     525   BIC:                             724.0
 Df Model:                          11                                         
@@ -418,7 +419,7 @@
 Model:                            OLS   Adj. R-squared:                  0.039
 Method:                 Least Squares   F-statistic:                     3.150
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):           0.000627
-Time:                        22:58:29   Log-Likelihood:                -325.29
+Time:                        23:07:16   Log-Likelihood:                -325.29
 No. Observations:                 537   AIC:                             672.6
 Df Residuals:                     526   BIC:                             719.7
 Df Model:                          10                                         
@@ -453,7 +454,7 @@
 Model:                            OLS   Adj. R-squared:                  0.036
 Method:                 Least Squares   F-statistic:                     3.196
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):           0.000885
-Time:                        22:58:29   Log-Likelihood:                -326.64
+Time:                        23:07:16   Log-Likelihood:                -326.64
 No. Observations:                 537   AIC:                             673.3
 Df Residuals:                     527   BIC:                             716.1
 Df Model:                           9                                         
@@ -487,7 +488,7 @@
 Model:                            OLS   Adj. R-squared:                  0.033
 Method:                 Least Squares   F-statistic:                     3.272
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00119
-Time:                        22:58:29   Log-Likelihood:                -327.92
+Time:                        23:07:16   Log-Likelihood:                -327.92
 No. Observations:                 537   AIC:                             673.8
 Df Residuals:                     528   BIC:                             712.4
 Df Model:                           8                                         
@@ -520,7 +521,7 @@
 Model:                            OLS   Adj. R-squared:                  0.028
 Method:                 Least Squares   F-statistic:                     3.243
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00222
-Time:                        22:58:29   Log-Likelihood:                -329.63
+Time:                        23:07:16   Log-Likelihood:                -329.63
 No. Observations:                 537   AIC:                             675.3
 Df Residuals:                     529   BIC:                             709.5
 Df Model:                           7                                         
@@ -552,7 +553,7 @@
 Model:                            OLS   Adj. R-squared:                  0.025
 Method:                 Least Squares   F-statistic:                     3.275
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00359
-Time:                        22:58:29   Log-Likelihood:                -331.13
+Time:                        23:07:16   Log-Likelihood:                -331.13
 No. Observations:                 537   AIC:                             676.3
 Df Residuals:                     530   BIC:                             706.3
 Df Model:                           6                                         
@@ -583,7 +584,7 @@
 Model:                            OLS   Adj. R-squared:                  0.022
 Method:                 Least Squares   F-statistic:                     3.428
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00466
-Time:                        22:58:29   Log-Likelihood:                -332.38
+Time:                        23:07:16   Log-Likelihood:                -332.38
 No. Observations:                 537   AIC:                             676.8
 Df Residuals:                     531   BIC:                             702.5
 Df Model:                           5                                         
@@ -609,11 +610,40 @@
   <si>
     <t xml:space="preserve">                            OLS Regression Results                            
 ==============================================================================
+Dep. Variable:               Desertor   R-squared:                       0.027
+Model:                            OLS   Adj. R-squared:                  0.020
+Method:                 Least Squares   F-statistic:                     3.730
+Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00527
+Time:                        23:07:16   Log-Likelihood:                -333.48
+No. Observations:                 537   AIC:                             677.0
+Df Residuals:                     532   BIC:                             698.4
+Df Model:                           4                                         
+Covariance Type:            nonrobust                                         
+=====================================================================================
+                        coef    std err          t      P&gt;|t|      [0.025      0.975]
+-------------------------------------------------------------------------------------
+Ones                  0.2551      0.095      2.698      0.007       0.069       0.441
+SchoolRegion_1       -0.2378      0.084     -2.822      0.005      -0.403      -0.072
+SchoolRegion_2       -0.1387      0.057     -2.414      0.016      -0.252      -0.026
+SchoolType_2          0.0964      0.073      1.318      0.188      -0.047       0.240
+PostulationType_1     0.1721      0.084      2.051      0.041       0.007       0.337
+==============================================================================
+Omnibus:                      271.153   Durbin-Watson:                   1.935
+Prob(Omnibus):                  0.000   Jarque-Bera (JB):               95.390
+Skew:                           0.864   Prob(JB):                     1.93e-21
+Kurtosis:                       1.870   Cond. No.                         10.4
+==============================================================================
+Warnings:
+[1] Standard Errors assume that the covariance matrix of the errors is correctly specified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            OLS Regression Results                            
+==============================================================================
 Dep. Variable:               Desertor   R-squared:                       0.024
 Model:                            OLS   Adj. R-squared:                  0.019
 Method:                 Least Squares   F-statistic:                     4.388
 Date:                Sun, 22 Dec 2019   Prob (F-statistic):            0.00460
-Time:                        22:58:29   Log-Likelihood:                -334.36
+Time:                        23:07:16   Log-Likelihood:                -334.36
 No. Observations:                 537   AIC:                             676.7
 Df Residuals:                     533   BIC:                             693.9
 Df Model:                           3                                         
@@ -1418,12 +1448,54 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="344.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="357" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="344.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>